<commit_message>
admittable errors in ricotta boiling plan
</commit_message>
<xml_diff>
--- a/app/data/inputs/ricotta/sample_boiling_plan.xlsx
+++ b/app/data/inputs/ricotta/sample_boiling_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenijkadaner/Yandex.Disk.localized/master/code/git/2020.10-umalat/umalat/app/data/inputs/ricotta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D550AE6-40CF-5546-A837-9C966705DAE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4842D160-302F-444D-A3D0-CA58DD71DC2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2359,18 +2359,15 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2387,6 +2384,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -46167,7 +46167,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>660</v>
       </c>
       <c r="B2" s="33" t="s">
@@ -46216,8 +46216,8 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="25" t="s">
         <v>175</v>
       </c>
@@ -46241,7 +46241,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>662</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -46412,8 +46412,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="25" t="s">
         <v>173</v>
       </c>
@@ -46437,7 +46437,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>664</v>
       </c>
       <c r="B15" s="33" t="s">
@@ -46483,8 +46483,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="25" t="s">
         <v>187</v>
       </c>
@@ -46508,7 +46508,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="34" t="s">
         <v>666</v>
       </c>
       <c r="B19" s="33" t="s">
@@ -46554,8 +46554,8 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="25" t="s">
         <v>179</v>
       </c>
@@ -46579,7 +46579,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="34" t="s">
         <v>668</v>
       </c>
       <c r="B23" s="33" t="s">
@@ -46625,8 +46625,8 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="25" t="s">
         <v>179</v>
       </c>
@@ -46650,7 +46650,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="34" t="s">
         <v>670</v>
       </c>
       <c r="B27" s="33" t="s">
@@ -46696,7 +46696,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="34" t="s">
         <v>672</v>
       </c>
       <c r="B30" s="33" t="s">
@@ -46743,6 +46743,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="B30"/>
     <mergeCell ref="A30"/>
     <mergeCell ref="B19:B20"/>
@@ -46751,12 +46757,6 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B27"/>
     <mergeCell ref="A27"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B6:B12"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -46772,8 +46772,8 @@
   <dimension ref="A1:AMK165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46801,38 +46801,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="45" t="s">
         <v>674</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="37" t="s">
         <v>649</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>675</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="37" t="s">
         <v>676</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="37" t="s">
         <v>677</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="37" t="s">
         <v>678</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="37" t="s">
         <v>679</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>680</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="41" t="s">
         <v>681</v>
       </c>
       <c r="J1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
-      <c r="Q1" s="44"/>
+      <c r="Q1" s="43"/>
       <c r="R1" s="15" t="s">
         <v>682</v>
       </c>
@@ -46851,8 +46851,8 @@
       <c r="E2" s="38"/>
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="43"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="14" t="s">
         <v>685</v>
       </c>
@@ -46865,7 +46865,7 @@
       <c r="N2" s="14">
         <v>0</v>
       </c>
-      <c r="Q2" s="45"/>
+      <c r="Q2" s="44"/>
       <c r="R2" s="27">
         <v>124740</v>
       </c>
@@ -46896,7 +46896,7 @@
         <v>282</v>
       </c>
       <c r="F3" s="28">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="G3" s="20" t="str">
         <f ca="1">IF(H3="", IF(J3="","",#REF!+(INDIRECT("N" &amp; ROW() - 1) - N3)),IF(J3="", "", INDIRECT("N" &amp; ROW() - 1) - N3))</f>
@@ -46909,7 +46909,7 @@
       <c r="I3" s="22"/>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K34" ca="1" si="2">IF(J3 = "-", -INDIRECT("C" &amp; ROW() - 1),F3)</f>
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L34" ca="1" si="3">IF(J3 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K3)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K3)))), 0)</f>
@@ -46943,7 +46943,7 @@
       </c>
       <c r="G4" s="20">
         <f ca="1">IF(H4="", IF(J4="","",#REF!+(INDIRECT("N" &amp; ROW() - 1) - N4)),IF(J4="", "", INDIRECT("N" &amp; ROW() - 1) - N4))</f>
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="H4" s="21">
         <f t="shared" ca="1" si="1"/>
@@ -46961,7 +46961,7 @@
       </c>
       <c r="L4" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" si="4"/>
@@ -46969,7 +46969,7 @@
       </c>
       <c r="N4" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47015,7 +47015,7 @@
       </c>
       <c r="N5" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47055,7 +47055,7 @@
       </c>
       <c r="L6" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="4"/>
@@ -47063,7 +47063,7 @@
       </c>
       <c r="N6" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47109,7 +47109,7 @@
       </c>
       <c r="N7" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47155,7 +47155,7 @@
       </c>
       <c r="N8" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47195,7 +47195,7 @@
       </c>
       <c r="L9" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" si="4"/>
@@ -47203,7 +47203,7 @@
       </c>
       <c r="N9" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47249,7 +47249,7 @@
       </c>
       <c r="N10" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47289,7 +47289,7 @@
       </c>
       <c r="L11" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M11" s="1">
         <f t="shared" si="4"/>
@@ -47297,7 +47297,7 @@
       </c>
       <c r="N11" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47343,7 +47343,7 @@
       </c>
       <c r="N12" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47383,7 +47383,7 @@
       </c>
       <c r="L13" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M13" s="1">
         <f t="shared" si="4"/>
@@ -47391,7 +47391,7 @@
       </c>
       <c r="N13" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47437,7 +47437,7 @@
       </c>
       <c r="N14" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47477,7 +47477,7 @@
       </c>
       <c r="L15" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M15" s="1">
         <f t="shared" si="4"/>
@@ -47485,7 +47485,7 @@
       </c>
       <c r="N15" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47531,7 +47531,7 @@
       </c>
       <c r="N16" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47571,7 +47571,7 @@
       </c>
       <c r="L17" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M17" s="1">
         <f t="shared" si="4"/>
@@ -47579,7 +47579,7 @@
       </c>
       <c r="N17" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47625,7 +47625,7 @@
       </c>
       <c r="N18" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47665,7 +47665,7 @@
       </c>
       <c r="L19" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M19" s="1">
         <f t="shared" si="4"/>
@@ -47673,7 +47673,7 @@
       </c>
       <c r="N19" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47719,7 +47719,7 @@
       </c>
       <c r="N20" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47759,7 +47759,7 @@
       </c>
       <c r="L21" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M21" s="1">
         <f t="shared" si="4"/>
@@ -47767,7 +47767,7 @@
       </c>
       <c r="N21" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47813,7 +47813,7 @@
       </c>
       <c r="N22" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47853,7 +47853,7 @@
       </c>
       <c r="L23" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M23" s="1">
         <f t="shared" si="4"/>
@@ -47861,7 +47861,7 @@
       </c>
       <c r="N23" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47907,7 +47907,7 @@
       </c>
       <c r="N24" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -47947,7 +47947,7 @@
       </c>
       <c r="L25" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M25" s="1">
         <f t="shared" si="4"/>
@@ -47955,7 +47955,7 @@
       </c>
       <c r="N25" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48001,7 +48001,7 @@
       </c>
       <c r="N26" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48041,7 +48041,7 @@
       </c>
       <c r="L27" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M27" s="1">
         <f t="shared" si="4"/>
@@ -48049,7 +48049,7 @@
       </c>
       <c r="N27" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48095,7 +48095,7 @@
       </c>
       <c r="N28" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48135,7 +48135,7 @@
       </c>
       <c r="L29" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M29" s="1">
         <f t="shared" si="4"/>
@@ -48143,7 +48143,7 @@
       </c>
       <c r="N29" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48189,7 +48189,7 @@
       </c>
       <c r="N30" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48229,7 +48229,7 @@
       </c>
       <c r="L31" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M31" s="1">
         <f t="shared" si="4"/>
@@ -48237,7 +48237,7 @@
       </c>
       <c r="N31" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48283,7 +48283,7 @@
       </c>
       <c r="N32" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48323,7 +48323,7 @@
       </c>
       <c r="L33" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M33" s="1">
         <f t="shared" si="4"/>
@@ -48331,7 +48331,7 @@
       </c>
       <c r="N33" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48377,7 +48377,7 @@
       </c>
       <c r="N34" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48417,7 +48417,7 @@
       </c>
       <c r="L35" s="1">
         <f t="shared" ref="L35:L66" ca="1" si="9">IF(J35 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K35)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K35)))), 0)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M35" s="1">
         <f t="shared" ref="M35:M66" si="10">IF(J35="-",1,0)</f>
@@ -48425,7 +48425,7 @@
       </c>
       <c r="N35" s="1">
         <f t="shared" ref="N35:N66" ca="1" si="11">IF(L35 = 0, INDIRECT("N" &amp; ROW() - 1), L35)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48471,7 +48471,7 @@
       </c>
       <c r="N36" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48511,7 +48511,7 @@
       </c>
       <c r="L37" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M37" s="1">
         <f t="shared" si="10"/>
@@ -48519,7 +48519,7 @@
       </c>
       <c r="N37" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48565,7 +48565,7 @@
       </c>
       <c r="N38" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48605,7 +48605,7 @@
       </c>
       <c r="L39" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M39" s="1">
         <f t="shared" si="10"/>
@@ -48613,7 +48613,7 @@
       </c>
       <c r="N39" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48659,7 +48659,7 @@
       </c>
       <c r="N40" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48699,7 +48699,7 @@
       </c>
       <c r="L41" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M41" s="1">
         <f t="shared" si="10"/>
@@ -48707,7 +48707,7 @@
       </c>
       <c r="N41" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48753,7 +48753,7 @@
       </c>
       <c r="N42" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48793,7 +48793,7 @@
       </c>
       <c r="L43" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M43" s="1">
         <f t="shared" si="10"/>
@@ -48801,7 +48801,7 @@
       </c>
       <c r="N43" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48847,7 +48847,7 @@
       </c>
       <c r="N44" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48893,7 +48893,7 @@
       </c>
       <c r="N45" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48933,7 +48933,7 @@
       </c>
       <c r="L46" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M46" s="1">
         <f t="shared" si="10"/>
@@ -48941,7 +48941,7 @@
       </c>
       <c r="N46" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -48987,7 +48987,7 @@
       </c>
       <c r="N47" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49027,7 +49027,7 @@
       </c>
       <c r="L48" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M48" s="1">
         <f t="shared" si="10"/>
@@ -49035,7 +49035,7 @@
       </c>
       <c r="N48" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49081,7 +49081,7 @@
       </c>
       <c r="N49" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49127,7 +49127,7 @@
       </c>
       <c r="N50" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49167,7 +49167,7 @@
       </c>
       <c r="L51" s="1">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M51" s="1">
         <f t="shared" si="10"/>
@@ -49175,7 +49175,7 @@
       </c>
       <c r="N51" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49202,7 +49202,7 @@
       </c>
       <c r="N52" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49229,7 +49229,7 @@
       </c>
       <c r="N53" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49256,7 +49256,7 @@
       </c>
       <c r="N54" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49283,7 +49283,7 @@
       </c>
       <c r="N55" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49310,7 +49310,7 @@
       </c>
       <c r="N56" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49337,7 +49337,7 @@
       </c>
       <c r="N57" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49364,7 +49364,7 @@
       </c>
       <c r="N58" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49391,7 +49391,7 @@
       </c>
       <c r="N59" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49418,7 +49418,7 @@
       </c>
       <c r="N60" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49445,7 +49445,7 @@
       </c>
       <c r="N61" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49472,7 +49472,7 @@
       </c>
       <c r="N62" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49499,7 +49499,7 @@
       </c>
       <c r="N63" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49526,7 +49526,7 @@
       </c>
       <c r="N64" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49553,7 +49553,7 @@
       </c>
       <c r="N65" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49580,7 +49580,7 @@
       </c>
       <c r="N66" s="1">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49598,7 +49598,7 @@
         <v>0</v>
       </c>
       <c r="L67" s="1">
-        <f t="shared" ref="L67:L98" ca="1" si="14">IF(J67 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K67)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K67)))), 0)</f>
+        <f t="shared" ref="L67:L74" ca="1" si="14">IF(J67 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K67)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K67)))), 0)</f>
         <v>0</v>
       </c>
       <c r="M67" s="1">
@@ -49607,7 +49607,7 @@
       </c>
       <c r="N67" s="1">
         <f t="shared" ref="N67:N98" ca="1" si="16">IF(L67 = 0, INDIRECT("N" &amp; ROW() - 1), L67)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49634,7 +49634,7 @@
       </c>
       <c r="N68" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49661,7 +49661,7 @@
       </c>
       <c r="N69" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49688,7 +49688,7 @@
       </c>
       <c r="N70" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49715,7 +49715,7 @@
       </c>
       <c r="N71" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49742,7 +49742,7 @@
       </c>
       <c r="N72" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49769,7 +49769,7 @@
       </c>
       <c r="N73" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49796,7 +49796,7 @@
       </c>
       <c r="N74" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49823,7 +49823,7 @@
       </c>
       <c r="N75" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49850,7 +49850,7 @@
       </c>
       <c r="N76" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49877,7 +49877,7 @@
       </c>
       <c r="N77" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49904,7 +49904,7 @@
       </c>
       <c r="N78" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49931,7 +49931,7 @@
       </c>
       <c r="N79" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49958,7 +49958,7 @@
       </c>
       <c r="N80" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -49985,7 +49985,7 @@
       </c>
       <c r="N81" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50012,7 +50012,7 @@
       </c>
       <c r="N82" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50039,7 +50039,7 @@
       </c>
       <c r="N83" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50066,7 +50066,7 @@
       </c>
       <c r="N84" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50093,7 +50093,7 @@
       </c>
       <c r="N85" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50120,7 +50120,7 @@
       </c>
       <c r="N86" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50147,7 +50147,7 @@
       </c>
       <c r="N87" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50174,7 +50174,7 @@
       </c>
       <c r="N88" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50201,7 +50201,7 @@
       </c>
       <c r="N89" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50228,7 +50228,7 @@
       </c>
       <c r="N90" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50255,7 +50255,7 @@
       </c>
       <c r="N91" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50282,7 +50282,7 @@
       </c>
       <c r="N92" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50309,7 +50309,7 @@
       </c>
       <c r="N93" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50336,7 +50336,7 @@
       </c>
       <c r="N94" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50363,7 +50363,7 @@
       </c>
       <c r="N95" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50390,7 +50390,7 @@
       </c>
       <c r="N96" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50417,7 +50417,7 @@
       </c>
       <c r="N97" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50444,7 +50444,7 @@
       </c>
       <c r="N98" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50458,7 +50458,7 @@
       </c>
       <c r="I99" s="22"/>
       <c r="K99" s="1">
-        <f t="shared" ref="K99:K130" ca="1" si="19">IF(J99 = "-", -INDIRECT("C" &amp; ROW() - 1),F99)</f>
+        <f t="shared" ref="K99:K123" ca="1" si="19">IF(J99 = "-", -INDIRECT("C" &amp; ROW() - 1),F99)</f>
         <v>0</v>
       </c>
       <c r="L99" s="1">
@@ -50471,7 +50471,7 @@
       </c>
       <c r="N99" s="1">
         <f t="shared" ref="N99:N123" ca="1" si="21">IF(L99 = 0, INDIRECT("N" &amp; ROW() - 1), L99)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50498,7 +50498,7 @@
       </c>
       <c r="N100" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50525,7 +50525,7 @@
       </c>
       <c r="N101" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50552,7 +50552,7 @@
       </c>
       <c r="N102" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50579,7 +50579,7 @@
       </c>
       <c r="N103" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50606,7 +50606,7 @@
       </c>
       <c r="N104" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50633,7 +50633,7 @@
       </c>
       <c r="N105" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50660,7 +50660,7 @@
       </c>
       <c r="N106" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50687,7 +50687,7 @@
       </c>
       <c r="N107" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50714,7 +50714,7 @@
       </c>
       <c r="N108" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50741,7 +50741,7 @@
       </c>
       <c r="N109" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50768,7 +50768,7 @@
       </c>
       <c r="N110" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50795,7 +50795,7 @@
       </c>
       <c r="N111" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50822,7 +50822,7 @@
       </c>
       <c r="N112" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50849,7 +50849,7 @@
       </c>
       <c r="N113" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50876,7 +50876,7 @@
       </c>
       <c r="N114" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50903,7 +50903,7 @@
       </c>
       <c r="N115" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50930,7 +50930,7 @@
       </c>
       <c r="N116" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50957,7 +50957,7 @@
       </c>
       <c r="N117" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -50984,7 +50984,7 @@
       </c>
       <c r="N118" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -51011,7 +51011,7 @@
       </c>
       <c r="N119" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -51038,7 +51038,7 @@
       </c>
       <c r="N120" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -51065,7 +51065,7 @@
       </c>
       <c r="N121" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -51092,7 +51092,7 @@
       </c>
       <c r="N122" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -51119,7 +51119,7 @@
       </c>
       <c r="N123" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="7:14" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -51376,16 +51376,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B123 B3:B5">
     <cfRule type="expression" dxfId="40" priority="2">

</xml_diff>